<commit_message>
Final update for Mini Project 2
</commit_message>
<xml_diff>
--- a/Part 2 - DASK and Datatypes/Computations Analysis.xlsx
+++ b/Part 2 - DASK and Datatypes/Computations Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukad\Documents\GitHub\Mandelbrot-Mini-Project\Part 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukad\Documents\GitHub\Mandelbrot-Mini-Project\Part 2 - DASK and Datatypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF9B88E-FCBA-43CD-86C0-1361B020EB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A8B466-F31C-4684-B27F-9BCE7C1743AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CEFBBC89-B58E-4E09-B71E-131FBE424AED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CEFBBC89-B58E-4E09-B71E-131FBE424AED}"/>
   </bookViews>
   <sheets>
     <sheet name="DASK NUMPY" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,29 @@
     <sheet name="DASK Distributed Chunk Sizes " sheetId="4" r:id="rId3"/>
     <sheet name="DASK Local Chunk Sizes" sheetId="1" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Data Types'!$N$6</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Data Types'!$N$6:$N$8</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Data Types'!$O$7</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'Data Types'!$O$7:$O$9</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'Data Types'!$O$7:$P$7</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'Data Types'!$P$5</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'Data Types'!$P$6:$P$8</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'Data Types'!$P$7:$P$9</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'Data Types'!$N$6:$N$8</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'Data Types'!$O$5</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'Data Types'!$O$6:$O$8</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'Data Types'!$P$5</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Data Types'!$N$6:$P$6</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'Data Types'!$P$6:$P$8</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Data Types'!$N$7:$N$9</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Data Types'!$O$5</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Data Types'!$O$5:$P$5</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Data Types'!$O$6</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Data Types'!$O$6:$O$8</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Data Types'!$O$6:$P$6</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Data Types'!$O$6:$P$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Chunk</t>
   </si>
@@ -61,12 +84,27 @@
   <si>
     <t>NUMPY</t>
   </si>
+  <si>
+    <t>Complex64</t>
+  </si>
+  <si>
+    <t>Complex128</t>
+  </si>
+  <si>
+    <t>Float32</t>
+  </si>
+  <si>
+    <t>Float64</t>
+  </si>
+  <si>
+    <t>Float16</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,16 +118,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -97,15 +154,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -246,7 +326,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4751,18 +4830,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC079FF6-B4E1-441D-AFED-DAF99CC11C2D}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4770,7 +4850,7 @@
         <v>193.15727000000001</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -4778,7 +4858,7 @@
         <v>189.50313</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -4786,7 +4866,61 @@
         <v>189.09297000000001</v>
       </c>
     </row>
+    <row r="5" spans="1:16" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="3"/>
+      <c r="O5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O6" s="2">
+        <v>155.1</v>
+      </c>
+      <c r="P6" s="2">
+        <v>193.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="2">
+        <v>157.76</v>
+      </c>
+      <c r="P7" s="2">
+        <v>199.54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="2">
+        <v>199.08</v>
+      </c>
+      <c r="P8" s="2">
+        <v>223.37</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="O6:P8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="9"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -4797,7 +4931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BFD5D2-3AEE-40ED-806F-B32A6FAABD73}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Mini Project Part 2 Hand-In
</commit_message>
<xml_diff>
--- a/Part 2 - DASK and Datatypes/Computations Analysis.xlsx
+++ b/Part 2 - DASK and Datatypes/Computations Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukad\Documents\GitHub\Mandelbrot-Mini-Project\Part 2 - DASK and Datatypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A8B466-F31C-4684-B27F-9BCE7C1743AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62AB831-9CCE-4BCF-8551-15372659DAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CEFBBC89-B58E-4E09-B71E-131FBE424AED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CEFBBC89-B58E-4E09-B71E-131FBE424AED}"/>
   </bookViews>
   <sheets>
     <sheet name="DASK NUMPY" sheetId="3" r:id="rId1"/>
@@ -18,29 +18,6 @@
     <sheet name="DASK Distributed Chunk Sizes " sheetId="4" r:id="rId3"/>
     <sheet name="DASK Local Chunk Sizes" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Data Types'!$N$6</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Data Types'!$N$6:$N$8</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Data Types'!$O$7</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Data Types'!$O$7:$O$9</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Data Types'!$O$7:$P$7</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Data Types'!$P$5</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Data Types'!$P$6:$P$8</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'Data Types'!$P$7:$P$9</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'Data Types'!$N$6:$N$8</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'Data Types'!$O$5</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'Data Types'!$O$6:$O$8</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'Data Types'!$P$5</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Data Types'!$N$6:$P$6</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'Data Types'!$P$6:$P$8</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Data Types'!$N$7:$N$9</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Data Types'!$O$5</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Data Types'!$O$5:$P$5</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Data Types'!$O$6</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Data Types'!$O$6:$O$8</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Data Types'!$O$6:$P$6</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Data Types'!$O$6:$P$8</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -104,6 +81,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,7 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -183,6 +163,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
@@ -310,11 +291,11 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>44.787999999999997</c:v>
+                <c:pt idx="0" formatCode="0.000">
+                  <c:v>53.89</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.685000000000002</c:v>
+                  <c:v>101.604</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -525,7 +506,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1292,16 +1273,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.0449999999999999</c:v>
+                  <c:v>3.1970000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8769999999999998</c:v>
+                  <c:v>8.57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.902999999999999</c:v>
+                  <c:v>30.077999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>102.74</c:v>
+                  <c:v>116.413</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1814,16 +1795,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.25</c:v>
+                  <c:v>2.6840000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.013999999999999</c:v>
+                  <c:v>11.852</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56.777999999999999</c:v>
+                  <c:v>50.335999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>262.04599999999999</c:v>
+                  <c:v>250.167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4800,8 +4781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C11E05E-2569-4320-B04C-83B4FF0CB242}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4810,8 +4791,8 @@
       <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1">
-        <v>44.787999999999997</v>
+      <c r="B1" s="4">
+        <v>53.89</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -4819,7 +4800,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>54.685000000000002</v>
+        <v>101.604</v>
       </c>
     </row>
   </sheetData>
@@ -4832,8 +4813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC079FF6-B4E1-441D-AFED-DAF99CC11C2D}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5:P8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4932,7 +4913,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4950,7 +4931,7 @@
         <v>500</v>
       </c>
       <c r="B2">
-        <v>2.0449999999999999</v>
+        <v>3.1970000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -4958,7 +4939,7 @@
         <v>200</v>
       </c>
       <c r="B3">
-        <v>6.8769999999999998</v>
+        <v>8.57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4966,7 +4947,7 @@
         <v>100</v>
       </c>
       <c r="B4">
-        <v>25.902999999999999</v>
+        <v>30.077999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4974,7 +4955,7 @@
         <v>50</v>
       </c>
       <c r="B5">
-        <v>102.74</v>
+        <v>116.413</v>
       </c>
     </row>
   </sheetData>
@@ -4988,7 +4969,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5006,7 +4987,7 @@
         <v>500</v>
       </c>
       <c r="B2">
-        <v>3.25</v>
+        <v>2.6840000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5014,7 +4995,7 @@
         <v>200</v>
       </c>
       <c r="B3">
-        <v>17.013999999999999</v>
+        <v>11.852</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5022,7 +5003,7 @@
         <v>100</v>
       </c>
       <c r="B4">
-        <v>56.777999999999999</v>
+        <v>50.335999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -5030,7 +5011,7 @@
         <v>50</v>
       </c>
       <c r="B5">
-        <v>262.04599999999999</v>
+        <v>250.167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>